<commit_message>
Fuels are closer to being usable .. added key decision variables and constraints for consuming on a supply curve Improved documentation Renamed the files responsible for generation technologies to be less vague (generators -> gen_tech) Updated biomass projects to not be resource limited. Their upper bound of dispatch is given by limits on the available fuel in the supply curve.
</commit_message>
<xml_diff>
--- a/model/test_dat/gen_data_test.xlsx
+++ b/model/test_dat/gen_data_test.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13120" windowHeight="15800" tabRatio="686" activeTab="4"/>
+    <workbookView xWindow="12000" yWindow="0" windowWidth="16800" windowHeight="11000" tabRatio="686"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="gen info" sheetId="1" r:id="rId1"/>
+    <sheet name="gen costs" sheetId="2" r:id="rId2"/>
+    <sheet name="ccs info" sheetId="3" r:id="rId3"/>
+    <sheet name="storage info" sheetId="4" r:id="rId4"/>
+    <sheet name="gen_energy" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
   <si>
     <t>generation_technology</t>
   </si>
@@ -228,8 +228,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="229">
+  <cellStyleXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -465,7 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="229">
+  <cellStyles count="263">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -580,6 +614,23 @@
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -694,6 +745,23 @@
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1025,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1477,7 +1545,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="G11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2">
         <v>0</v>
@@ -1518,7 +1586,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="G12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2">
         <v>0</v>
@@ -1798,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1916,201 +1984,201 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
-        <v>29</v>
+      <c r="A7" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B7">
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>2687700</v>
+        <v>1143900</v>
       </c>
       <c r="D7">
-        <v>21390</v>
+        <v>5868.3</v>
       </c>
       <c r="E7">
-        <v>3.4502999999999999</v>
+        <v>3.4131</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>29</v>
+      <c r="A8" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B8">
         <v>2030</v>
       </c>
       <c r="C8">
-        <v>2687700</v>
+        <v>1143900</v>
       </c>
       <c r="D8">
-        <v>21390</v>
+        <v>5868.3</v>
       </c>
       <c r="E8">
-        <v>3.4502999999999999</v>
+        <v>3.4131</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="C9">
-        <v>1143900</v>
+        <v>3487500</v>
       </c>
       <c r="D9">
-        <v>5868.3</v>
+        <v>17112</v>
       </c>
       <c r="E9">
-        <v>3.4131</v>
+        <v>9.3000000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B10">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="C10">
-        <v>1143900</v>
+        <v>605430</v>
       </c>
       <c r="D10">
-        <v>5868.3</v>
+        <v>4891.8</v>
       </c>
       <c r="E10">
-        <v>3.4131</v>
+        <v>27.806999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>2030</v>
       </c>
       <c r="C11">
-        <v>3487500</v>
+        <v>605430</v>
       </c>
       <c r="D11">
-        <v>17112</v>
+        <v>4891.8</v>
       </c>
       <c r="E11">
-        <v>9.3000000000000007</v>
+        <v>27.806999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>2020</v>
+        <v>2030</v>
       </c>
       <c r="C12">
-        <v>605430</v>
+        <v>5673000</v>
       </c>
       <c r="D12">
-        <v>4891.8</v>
+        <v>118110</v>
       </c>
       <c r="E12">
-        <v>27.806999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="C13">
-        <v>605430</v>
+        <v>3561900</v>
       </c>
       <c r="D13">
-        <v>4891.8</v>
+        <v>88350</v>
       </c>
       <c r="E13">
-        <v>27.806999999999999</v>
+        <v>13.95</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>2030</v>
       </c>
       <c r="C14">
-        <v>5673000</v>
+        <v>3561900</v>
       </c>
       <c r="D14">
-        <v>118110</v>
+        <v>88350</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>13.95</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
+      <c r="A15" t="s">
+        <v>22</v>
       </c>
       <c r="B15">
+        <v>2030</v>
+      </c>
+      <c r="C15">
+        <v>5970600</v>
+      </c>
+      <c r="D15">
+        <v>100719</v>
+      </c>
+      <c r="E15">
+        <v>20.130700000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
         <v>2020</v>
       </c>
-      <c r="C15">
-        <v>3561900</v>
-      </c>
-      <c r="D15">
-        <v>88350</v>
-      </c>
-      <c r="E15">
-        <v>13.95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>2030</v>
-      </c>
       <c r="C16">
-        <v>3561900</v>
+        <v>3487500</v>
       </c>
       <c r="D16">
-        <v>88350</v>
+        <v>41850</v>
       </c>
       <c r="E16">
-        <v>13.95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>22</v>
+      <c r="A17" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B17">
         <v>2030</v>
       </c>
       <c r="C17">
-        <v>5970600</v>
+        <v>3059700</v>
       </c>
       <c r="D17">
-        <v>100719</v>
+        <v>38130</v>
       </c>
       <c r="E17">
-        <v>20.130700000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>2020</v>
       </c>
       <c r="C18">
-        <v>3487500</v>
+        <v>3106200</v>
       </c>
       <c r="D18">
         <v>41850</v>
@@ -2121,13 +2189,13 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>2030</v>
       </c>
       <c r="C19">
-        <v>3059700</v>
+        <v>2752800</v>
       </c>
       <c r="D19">
         <v>38130</v>
@@ -2138,13 +2206,13 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>2020</v>
       </c>
       <c r="C20">
-        <v>3106200</v>
+        <v>2334300</v>
       </c>
       <c r="D20">
         <v>41850</v>
@@ -2154,14 +2222,14 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>18</v>
+      <c r="A21" t="s">
+        <v>19</v>
       </c>
       <c r="B21">
         <v>2030</v>
       </c>
       <c r="C21">
-        <v>2752800</v>
+        <v>2148300</v>
       </c>
       <c r="D21">
         <v>38130</v>
@@ -2172,16 +2240,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>2020</v>
       </c>
       <c r="C22">
-        <v>2334300</v>
+        <v>1841400</v>
       </c>
       <c r="D22">
-        <v>41850</v>
+        <v>55800</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2189,16 +2257,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>2030</v>
       </c>
       <c r="C23">
-        <v>2148300</v>
+        <v>1841400</v>
       </c>
       <c r="D23">
-        <v>38130</v>
+        <v>55800</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2206,103 +2274,69 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B24">
         <v>2020</v>
       </c>
       <c r="C24">
-        <v>1841400</v>
+        <v>763417</v>
       </c>
       <c r="D24">
-        <v>55800</v>
+        <v>10788</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1.4415</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B25">
         <v>2030</v>
       </c>
       <c r="C25">
-        <v>1841400</v>
+        <v>763417</v>
       </c>
       <c r="D25">
-        <v>55800</v>
+        <v>10788</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1.4415</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>2020</v>
       </c>
       <c r="C26">
-        <v>763417</v>
+        <v>948188</v>
       </c>
       <c r="D26">
-        <v>10788</v>
+        <v>23436</v>
       </c>
       <c r="E26">
-        <v>1.4415</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>2030</v>
       </c>
       <c r="C27">
-        <v>763417</v>
+        <v>880287</v>
       </c>
       <c r="D27">
-        <v>10788</v>
+        <v>23436</v>
       </c>
       <c r="E27">
-        <v>1.4415</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28">
-        <v>2020</v>
-      </c>
-      <c r="C28">
-        <v>948188</v>
-      </c>
-      <c r="D28">
-        <v>23436</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29">
-        <v>2030</v>
-      </c>
-      <c r="C29">
-        <v>880287</v>
-      </c>
-      <c r="D29">
-        <v>23436</v>
-      </c>
-      <c r="E29">
         <v>0</v>
       </c>
     </row>
@@ -2515,7 +2549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="A1:B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Regressed partially implemented feature of allowing independent dispatch of each project build (aka project vintage) to make merging code easier. It still seems like a nice feature, but I don't have an immediate compelling reason to implement it.
Finished implementing the project_dispatch module with a unit test.

Added a sandbox test of the Pyomo Expression object and confirms that it can replace a derived variable.
</commit_message>
<xml_diff>
--- a/model/test_dat/gen_data_test.xlsx
+++ b/model/test_dat/gen_data_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="0" windowWidth="16800" windowHeight="11000" tabRatio="686"/>
+    <workbookView xWindow="1580" yWindow="400" windowWidth="27200" windowHeight="15580" tabRatio="686"/>
   </bookViews>
   <sheets>
     <sheet name="gen info" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="50">
   <si>
     <t>generation_technology</t>
   </si>
@@ -228,8 +228,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="263">
+  <cellStyleXfs count="303">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -499,7 +539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="263">
+  <cellStyles count="303">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -631,6 +671,26 @@
     <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -762,6 +822,26 @@
     <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1091,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD12"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1115,7 +1195,7 @@
     <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1155,8 +1235,11 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1196,8 +1279,11 @@
       <c r="M2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2">
+        <v>28.83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
         <v>14</v>
       </c>
@@ -1237,8 +1323,11 @@
       <c r="M3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3">
+        <v>6.0822000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -1278,8 +1367,11 @@
       <c r="M4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4">
+        <v>9.8580000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
@@ -1319,8 +1411,11 @@
       <c r="M5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5">
+        <v>3.4502999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
@@ -1360,8 +1455,11 @@
       <c r="M6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6" s="2">
+        <v>27.806999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1401,8 +1499,11 @@
       <c r="M7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7">
+        <v>3.4131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1442,8 +1543,11 @@
       <c r="M8" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -1483,8 +1587,11 @@
       <c r="M9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9">
+        <v>27.806999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1524,8 +1631,11 @@
       <c r="M10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1565,8 +1675,11 @@
       <c r="M11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11">
+        <v>13.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1606,8 +1719,11 @@
       <c r="M12" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12">
+        <v>20.130700000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1647,8 +1763,11 @@
       <c r="M13" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1688,8 +1807,11 @@
       <c r="M14" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -1729,8 +1851,11 @@
       <c r="M15" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1770,8 +1895,11 @@
       <c r="M16" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
         <v>39</v>
       </c>
@@ -1811,8 +1939,11 @@
       <c r="M17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17">
+        <v>1.4415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1852,6 +1983,60 @@
       <c r="M18" s="2">
         <v>0</v>
       </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1"/>
+      <c r="B39"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1"/>
+      <c r="B41"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43"/>
+      <c r="B43"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45"/>
+      <c r="B45"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47"/>
+      <c r="B47"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49"/>
+      <c r="B49"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1869,7 +2054,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:E10"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>